<commit_message>
ran test on different excel file. new reports
</commit_message>
<xml_diff>
--- a/TestData/qcTest - Copy.xlsx
+++ b/TestData/qcTest - Copy.xlsx
@@ -89,7 +89,7 @@
       <u val="single"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="14">
     <fill>
       <patternFill/>
     </fill>
@@ -156,6 +156,18 @@
         <bgColor rgb="00FFADB0"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFADB0"/>
+        <bgColor rgb="FFFFADB0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFADD8E6"/>
+        <bgColor rgb="FFADD8E6"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -169,7 +181,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="158">
+  <cellXfs count="187">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -464,6 +476,65 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="1" fillId="12" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="12" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="12" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="170" fontId="3" fillId="12" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="173" fontId="2" fillId="12" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="173" fontId="2" fillId="13" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="3" fillId="13" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="12" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="12" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -9526,173 +9597,184 @@
       <c r="AE103" s="139" t="n"/>
     </row>
     <row r="104" ht="15" customHeight="1">
-      <c r="A104" s="18" t="inlineStr">
+      <c r="A104" s="158" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B104" s="10" t="n">
+      <c r="B104" s="159" t="n">
         <v>13402</v>
       </c>
-      <c r="C104" s="18" t="n"/>
-      <c r="D104" s="18" t="n"/>
-      <c r="E104" s="18" t="n"/>
-      <c r="F104" s="18" t="inlineStr">
+      <c r="C104" s="158" t="n"/>
+      <c r="D104" s="158" t="n"/>
+      <c r="E104" s="158" t="n"/>
+      <c r="F104" s="158" t="inlineStr">
         <is>
           <t>John F. Kelly Stanley Electric generator booklet with negatives</t>
         </is>
       </c>
-      <c r="G104" s="18" t="n"/>
-      <c r="H104" s="18" t="inlineStr">
+      <c r="G104" s="158" t="n"/>
+      <c r="H104" s="158" t="inlineStr">
         <is>
           <t>John F. Kelly, Stanley Electric Manufacturing Generator Booklet, Inludes Negatives, 1896</t>
         </is>
       </c>
-      <c r="I104" s="18" t="inlineStr">
+      <c r="I104" s="158" t="inlineStr">
         <is>
           <t>Stanley Electric Manufacturing Company (Pittsfield, Mass.)</t>
         </is>
       </c>
-      <c r="J104" s="18" t="n"/>
-      <c r="K104" s="18" t="n"/>
-      <c r="L104" s="18" t="n"/>
-      <c r="N104" s="18" t="n"/>
-      <c r="O104" s="10" t="n">
+      <c r="J104" s="158" t="n"/>
+      <c r="K104" s="158" t="n"/>
+      <c r="L104" s="158" t="n"/>
+      <c r="M104" s="160" t="n"/>
+      <c r="N104" s="158" t="n"/>
+      <c r="O104" s="159" t="n">
         <v>1896</v>
       </c>
-      <c r="P104" s="13" t="inlineStr">
+      <c r="P104" s="161" t="inlineStr">
         <is>
           <t>1896-02-01</t>
         </is>
       </c>
-      <c r="Q104" s="18" t="n"/>
-      <c r="R104" s="18" t="inlineStr">
+      <c r="Q104" s="158" t="n"/>
+      <c r="R104" s="158" t="inlineStr">
         <is>
           <t xml:space="preserve">No Copyright - United States </t>
         </is>
       </c>
-      <c r="S104" s="18" t="inlineStr">
+      <c r="S104" s="158" t="inlineStr">
         <is>
           <t>78 Pages, 6 unscanned blank end pages</t>
         </is>
       </c>
-      <c r="T104" s="18" t="inlineStr">
+      <c r="T104" s="158" t="inlineStr">
         <is>
           <t>Box 4 Folder 2 (job name lists folder 1</t>
         </is>
       </c>
-      <c r="U104" s="17" t="inlineStr">
+      <c r="U104" s="162" t="inlineStr">
         <is>
           <t>Becky to Scan</t>
         </is>
       </c>
-      <c r="V104" s="18" t="inlineStr">
+      <c r="V104" s="158" t="inlineStr">
         <is>
           <t>ZWU_SCA0319.B04.F02</t>
         </is>
       </c>
-      <c r="W104" s="41" t="n">
+      <c r="W104" s="163" t="n">
         <v>45448</v>
       </c>
-      <c r="X104" s="18" t="inlineStr">
+      <c r="X104" s="158" t="inlineStr">
         <is>
           <t>RF</t>
         </is>
       </c>
-      <c r="Y104" s="99" t="inlineStr">
+      <c r="Y104" s="164" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
       </c>
-      <c r="Z104" s="99" t="inlineStr">
+      <c r="Z104" s="164" t="inlineStr">
         <is>
           <t>MC</t>
         </is>
       </c>
-      <c r="AB104" s="99" t="inlineStr">
+      <c r="AA104" s="160" t="n"/>
+      <c r="AB104" s="164" t="inlineStr">
         <is>
           <t xml:space="preserve">F01_Neg and System Numbers to be interwoven into Zeus. when complete </t>
         </is>
       </c>
+      <c r="AC104" s="160" t="n"/>
+      <c r="AD104" s="160" t="n"/>
+      <c r="AE104" s="160" t="n"/>
     </row>
     <row r="105" ht="90" customHeight="1">
-      <c r="A105" s="18" t="inlineStr">
+      <c r="A105" s="158" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B105" s="10" t="n">
+      <c r="B105" s="159" t="n">
         <v>13243</v>
       </c>
-      <c r="C105" s="18" t="n"/>
-      <c r="D105" s="18" t="n"/>
-      <c r="E105" s="18" t="n"/>
-      <c r="F105" s="18" t="inlineStr">
+      <c r="C105" s="158" t="n"/>
+      <c r="D105" s="158" t="n"/>
+      <c r="E105" s="158" t="n"/>
+      <c r="F105" s="158" t="inlineStr">
         <is>
           <t>Shipping Order Book</t>
         </is>
       </c>
-      <c r="H105" s="18" t="inlineStr">
+      <c r="G105" s="160" t="n"/>
+      <c r="H105" s="158" t="inlineStr">
         <is>
           <t>Stanley Electric Manufacturing Company, Shipping Order Book, June 3, 1895 to July 31, 1895</t>
         </is>
       </c>
-      <c r="I105" s="18" t="inlineStr">
+      <c r="I105" s="158" t="inlineStr">
         <is>
           <t>Stanley Electric Manufacturing Company (Pittsfield, Mass.)</t>
         </is>
       </c>
-      <c r="J105" s="18" t="n"/>
-      <c r="K105" s="18" t="n"/>
-      <c r="L105" s="18" t="n"/>
-      <c r="M105" s="18" t="n"/>
-      <c r="N105" s="10" t="n"/>
-      <c r="O105" s="10" t="inlineStr">
+      <c r="J105" s="158" t="n"/>
+      <c r="K105" s="158" t="n"/>
+      <c r="L105" s="158" t="n"/>
+      <c r="M105" s="158" t="n"/>
+      <c r="N105" s="159" t="n"/>
+      <c r="O105" s="159" t="inlineStr">
         <is>
           <t>1895-06-03 to 1895-07-31</t>
         </is>
       </c>
-      <c r="P105" s="10" t="n"/>
-      <c r="Q105" s="18" t="n"/>
-      <c r="R105" s="18" t="inlineStr">
+      <c r="P105" s="159" t="n"/>
+      <c r="Q105" s="158" t="n"/>
+      <c r="R105" s="158" t="inlineStr">
         <is>
           <t xml:space="preserve">No Copyright - United States </t>
         </is>
       </c>
-      <c r="S105" s="18" t="n"/>
-      <c r="T105" s="17" t="inlineStr">
+      <c r="S105" s="158" t="n"/>
+      <c r="T105" s="162" t="inlineStr">
         <is>
           <t>Box 4 Folder 1 (file names need to be fixed to folder 1, currently folder 2 because job name entered wrong)</t>
         </is>
       </c>
-      <c r="U105" s="17" t="inlineStr">
+      <c r="U105" s="162" t="inlineStr">
         <is>
           <t>DO NOT FINALIZE Make sure to adjuest scan bed, glass down manually (do not lock glass in place using arrows on scanner)</t>
         </is>
       </c>
-      <c r="V105" s="18" t="inlineStr">
+      <c r="V105" s="158" t="inlineStr">
         <is>
           <t>ZWU_SCA0319.B04.F01</t>
         </is>
       </c>
-      <c r="W105" s="41" t="n">
+      <c r="W105" s="163" t="n">
         <v>45478</v>
       </c>
-      <c r="X105" s="18" t="inlineStr">
+      <c r="X105" s="158" t="inlineStr">
         <is>
           <t>KR, RB, MW, GH, MS, SK, JG</t>
         </is>
       </c>
-      <c r="Y105" s="99" t="inlineStr">
+      <c r="Y105" s="164" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
       </c>
-      <c r="Z105" s="99" t="inlineStr">
+      <c r="Z105" s="164" t="inlineStr">
         <is>
           <t>MC</t>
         </is>
       </c>
+      <c r="AA105" s="160" t="n"/>
+      <c r="AB105" s="160" t="n"/>
+      <c r="AC105" s="160" t="n"/>
+      <c r="AD105" s="160" t="n"/>
+      <c r="AE105" s="160" t="n"/>
     </row>
     <row r="106" ht="15" customHeight="1">
       <c r="A106" s="18" t="n"/>
@@ -20098,87 +20180,87 @@
       <c r="AE6" s="68" t="n"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="143" t="inlineStr">
+      <c r="A7" s="165" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B7" s="144" t="n">
+      <c r="B7" s="166" t="n">
         <v>13244</v>
       </c>
-      <c r="C7" s="145" t="n"/>
-      <c r="D7" s="145" t="n"/>
-      <c r="E7" s="145" t="n"/>
-      <c r="F7" s="146" t="inlineStr">
+      <c r="C7" s="167" t="n"/>
+      <c r="D7" s="167" t="n"/>
+      <c r="E7" s="167" t="n"/>
+      <c r="F7" s="168" t="inlineStr">
         <is>
           <t>S.K.C. Generator negatives and photographs</t>
         </is>
       </c>
-      <c r="G7" s="145" t="n"/>
-      <c r="H7" s="147" t="inlineStr">
+      <c r="G7" s="167" t="n"/>
+      <c r="H7" s="169" t="inlineStr">
         <is>
           <t xml:space="preserve">First S.K.C Generator made by Stanley Electric Mfg. Co., 1893, photograph </t>
         </is>
       </c>
-      <c r="I7" s="146" t="inlineStr">
+      <c r="I7" s="168" t="inlineStr">
         <is>
           <t>Stanley Electric Manufacturing Company (Pittsfield, Mass.)</t>
         </is>
       </c>
-      <c r="J7" s="145" t="n"/>
-      <c r="K7" s="145" t="n"/>
-      <c r="L7" s="145" t="n"/>
-      <c r="M7" s="145" t="n"/>
-      <c r="N7" s="145" t="n"/>
-      <c r="O7" s="145" t="n"/>
-      <c r="P7" s="148" t="n">
+      <c r="J7" s="167" t="n"/>
+      <c r="K7" s="167" t="n"/>
+      <c r="L7" s="167" t="n"/>
+      <c r="M7" s="167" t="n"/>
+      <c r="N7" s="167" t="n"/>
+      <c r="O7" s="167" t="n"/>
+      <c r="P7" s="170" t="n">
         <v>1893</v>
       </c>
-      <c r="Q7" s="145" t="n"/>
-      <c r="R7" s="137" t="inlineStr">
+      <c r="Q7" s="167" t="n"/>
+      <c r="R7" s="158" t="inlineStr">
         <is>
           <t>No Known Copyright</t>
         </is>
       </c>
-      <c r="S7" s="145" t="n"/>
-      <c r="T7" s="145" t="inlineStr">
+      <c r="S7" s="167" t="n"/>
+      <c r="T7" s="167" t="inlineStr">
         <is>
           <t>Box 5 Folder 1 Item 2</t>
         </is>
       </c>
-      <c r="U7" s="146" t="inlineStr">
+      <c r="U7" s="168" t="inlineStr">
         <is>
           <t>Glass Down, Leave in Sleeve</t>
         </is>
       </c>
-      <c r="V7" s="145" t="inlineStr">
+      <c r="V7" s="167" t="inlineStr">
         <is>
           <t>ZWU_SCA0319.B05.F01.06</t>
         </is>
       </c>
-      <c r="W7" s="149" t="n">
+      <c r="W7" s="171" t="n">
         <v>45496</v>
       </c>
-      <c r="X7" s="145" t="inlineStr">
+      <c r="X7" s="167" t="inlineStr">
         <is>
           <t>JG, SK</t>
         </is>
       </c>
-      <c r="Y7" s="141" t="inlineStr">
+      <c r="Y7" s="164" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
       </c>
-      <c r="Z7" s="145" t="inlineStr">
+      <c r="Z7" s="167" t="inlineStr">
         <is>
           <t>MC</t>
         </is>
       </c>
-      <c r="AA7" s="145" t="n"/>
-      <c r="AB7" s="145" t="n"/>
-      <c r="AC7" s="145" t="n"/>
-      <c r="AD7" s="145" t="n"/>
-      <c r="AE7" s="145" t="n"/>
+      <c r="AA7" s="167" t="n"/>
+      <c r="AB7" s="167" t="n"/>
+      <c r="AC7" s="167" t="n"/>
+      <c r="AD7" s="167" t="n"/>
+      <c r="AE7" s="167" t="n"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="114" t="inlineStr">
@@ -21830,676 +21912,676 @@
       <c r="AE26" s="68" t="n"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="143" t="inlineStr">
+      <c r="A27" s="165" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B27" s="144" t="n">
+      <c r="B27" s="166" t="n">
         <v>13250</v>
       </c>
-      <c r="C27" s="145" t="n"/>
-      <c r="D27" s="145" t="n"/>
-      <c r="E27" s="145" t="n"/>
-      <c r="F27" s="146" t="inlineStr">
+      <c r="C27" s="167" t="n"/>
+      <c r="D27" s="167" t="n"/>
+      <c r="E27" s="167" t="n"/>
+      <c r="F27" s="168" t="inlineStr">
         <is>
           <t>Induction meter documents and photographs</t>
         </is>
       </c>
-      <c r="G27" s="145" t="n"/>
-      <c r="H27" s="147" t="inlineStr">
+      <c r="G27" s="167" t="n"/>
+      <c r="H27" s="169" t="inlineStr">
         <is>
           <t>Photograph of Induction Meter, Undated 03</t>
         </is>
       </c>
-      <c r="I27" s="147" t="inlineStr">
+      <c r="I27" s="169" t="inlineStr">
         <is>
           <t>Stanley Instrument Co. (Gt. Barrington, Mass)</t>
         </is>
       </c>
-      <c r="J27" s="145" t="n"/>
-      <c r="K27" s="145" t="n"/>
-      <c r="L27" s="145" t="n"/>
-      <c r="M27" s="144" t="n">
+      <c r="J27" s="167" t="n"/>
+      <c r="K27" s="167" t="n"/>
+      <c r="L27" s="167" t="n"/>
+      <c r="M27" s="166" t="n">
         <v>1902</v>
       </c>
-      <c r="N27" s="145" t="n"/>
-      <c r="O27" s="145" t="inlineStr">
+      <c r="N27" s="167" t="n"/>
+      <c r="O27" s="167" t="inlineStr">
         <is>
           <t>undated</t>
         </is>
       </c>
-      <c r="P27" s="145" t="n"/>
-      <c r="Q27" s="145" t="n"/>
-      <c r="R27" s="137" t="inlineStr">
+      <c r="P27" s="167" t="n"/>
+      <c r="Q27" s="167" t="n"/>
+      <c r="R27" s="158" t="inlineStr">
         <is>
           <t xml:space="preserve">Copyright Undetermined </t>
         </is>
       </c>
-      <c r="S27" s="145" t="n"/>
-      <c r="T27" s="145" t="inlineStr">
+      <c r="S27" s="167" t="n"/>
+      <c r="T27" s="167" t="inlineStr">
         <is>
           <t>Box 5 Folder 9 Item 3</t>
         </is>
       </c>
-      <c r="U27" s="147" t="inlineStr">
+      <c r="U27" s="169" t="inlineStr">
         <is>
           <t xml:space="preserve">Glass Down, Leave in Sleeve </t>
         </is>
       </c>
-      <c r="V27" s="145" t="inlineStr">
+      <c r="V27" s="167" t="inlineStr">
         <is>
           <t>ZWU_SCA0319.B05.F09.02</t>
         </is>
       </c>
-      <c r="W27" s="149" t="n">
+      <c r="W27" s="171" t="n">
         <v>45497</v>
       </c>
-      <c r="X27" s="145" t="inlineStr">
+      <c r="X27" s="167" t="inlineStr">
         <is>
           <t>JG, SK</t>
         </is>
       </c>
-      <c r="Y27" s="141" t="inlineStr">
+      <c r="Y27" s="164" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
       </c>
-      <c r="Z27" s="145" t="inlineStr">
+      <c r="Z27" s="167" t="inlineStr">
         <is>
           <t>MC</t>
         </is>
       </c>
-      <c r="AA27" s="145" t="n"/>
-      <c r="AB27" s="145" t="n"/>
-      <c r="AC27" s="145" t="n"/>
-      <c r="AD27" s="145" t="n"/>
-      <c r="AE27" s="145" t="n"/>
+      <c r="AA27" s="167" t="n"/>
+      <c r="AB27" s="167" t="n"/>
+      <c r="AC27" s="167" t="n"/>
+      <c r="AD27" s="167" t="n"/>
+      <c r="AE27" s="167" t="n"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="143" t="inlineStr">
+      <c r="A28" s="165" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B28" s="144" t="n">
+      <c r="B28" s="166" t="n">
         <v>13250</v>
       </c>
-      <c r="C28" s="145" t="n"/>
-      <c r="D28" s="145" t="n"/>
-      <c r="E28" s="145" t="n"/>
-      <c r="F28" s="146" t="inlineStr">
+      <c r="C28" s="167" t="n"/>
+      <c r="D28" s="167" t="n"/>
+      <c r="E28" s="167" t="n"/>
+      <c r="F28" s="168" t="inlineStr">
         <is>
           <t>Induction meter documents and photographs</t>
         </is>
       </c>
-      <c r="G28" s="145" t="n"/>
-      <c r="H28" s="147" t="inlineStr">
+      <c r="G28" s="167" t="n"/>
+      <c r="H28" s="169" t="inlineStr">
         <is>
           <t xml:space="preserve">Photograph of Induction Meter, Undated , 04 </t>
         </is>
       </c>
-      <c r="I28" s="147" t="inlineStr">
+      <c r="I28" s="169" t="inlineStr">
         <is>
           <t>Stanley Instrument Co. (Gt. Barrington, Mass)</t>
         </is>
       </c>
-      <c r="J28" s="145" t="n"/>
-      <c r="K28" s="145" t="n"/>
-      <c r="L28" s="145" t="n"/>
-      <c r="M28" s="144" t="n">
+      <c r="J28" s="167" t="n"/>
+      <c r="K28" s="167" t="n"/>
+      <c r="L28" s="167" t="n"/>
+      <c r="M28" s="166" t="n">
         <v>1902</v>
       </c>
-      <c r="N28" s="145" t="n"/>
-      <c r="O28" s="145" t="inlineStr">
+      <c r="N28" s="167" t="n"/>
+      <c r="O28" s="167" t="inlineStr">
         <is>
           <t>undated</t>
         </is>
       </c>
-      <c r="P28" s="145" t="n"/>
-      <c r="Q28" s="145" t="n"/>
-      <c r="R28" s="137" t="inlineStr">
+      <c r="P28" s="167" t="n"/>
+      <c r="Q28" s="167" t="n"/>
+      <c r="R28" s="158" t="inlineStr">
         <is>
           <t xml:space="preserve">Copyright Undetermined </t>
         </is>
       </c>
-      <c r="S28" s="145" t="n"/>
-      <c r="T28" s="145" t="inlineStr">
+      <c r="S28" s="167" t="n"/>
+      <c r="T28" s="167" t="inlineStr">
         <is>
           <t>Box 5 Folder 9 Item 4</t>
         </is>
       </c>
-      <c r="U28" s="147" t="inlineStr">
+      <c r="U28" s="169" t="inlineStr">
         <is>
           <t xml:space="preserve">Glass Down, Leave in Sleeve </t>
         </is>
       </c>
-      <c r="V28" s="145" t="inlineStr">
+      <c r="V28" s="167" t="inlineStr">
         <is>
           <t>ZWU_SCA0319.B05.F09.03</t>
         </is>
       </c>
-      <c r="W28" s="149" t="n">
+      <c r="W28" s="171" t="n">
         <v>45497</v>
       </c>
-      <c r="X28" s="145" t="inlineStr">
+      <c r="X28" s="167" t="inlineStr">
         <is>
           <t>JG, SK</t>
         </is>
       </c>
-      <c r="Y28" s="141" t="inlineStr">
+      <c r="Y28" s="164" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
       </c>
-      <c r="Z28" s="145" t="inlineStr">
+      <c r="Z28" s="167" t="inlineStr">
         <is>
           <t>MC</t>
         </is>
       </c>
-      <c r="AA28" s="145" t="n"/>
-      <c r="AB28" s="145" t="n"/>
-      <c r="AC28" s="145" t="n"/>
-      <c r="AD28" s="145" t="n"/>
-      <c r="AE28" s="145" t="n"/>
+      <c r="AA28" s="167" t="n"/>
+      <c r="AB28" s="167" t="n"/>
+      <c r="AC28" s="167" t="n"/>
+      <c r="AD28" s="167" t="n"/>
+      <c r="AE28" s="167" t="n"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="143" t="inlineStr">
+      <c r="A29" s="165" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B29" s="144" t="n">
+      <c r="B29" s="166" t="n">
         <v>13250</v>
       </c>
-      <c r="C29" s="145" t="n"/>
-      <c r="D29" s="145" t="n"/>
-      <c r="E29" s="145" t="n"/>
-      <c r="F29" s="146" t="inlineStr">
+      <c r="C29" s="167" t="n"/>
+      <c r="D29" s="167" t="n"/>
+      <c r="E29" s="167" t="n"/>
+      <c r="F29" s="168" t="inlineStr">
         <is>
           <t>Induction meter documents and photographs</t>
         </is>
       </c>
-      <c r="G29" s="145" t="n"/>
-      <c r="H29" s="147" t="inlineStr">
+      <c r="G29" s="167" t="n"/>
+      <c r="H29" s="169" t="inlineStr">
         <is>
           <t>Photograph of Induction Meter, Undated  05</t>
         </is>
       </c>
-      <c r="I29" s="145" t="n"/>
-      <c r="J29" s="145" t="n"/>
-      <c r="K29" s="145" t="n"/>
-      <c r="L29" s="145" t="n"/>
-      <c r="M29" s="144" t="n">
+      <c r="I29" s="167" t="n"/>
+      <c r="J29" s="167" t="n"/>
+      <c r="K29" s="167" t="n"/>
+      <c r="L29" s="167" t="n"/>
+      <c r="M29" s="166" t="n">
         <v>1902</v>
       </c>
-      <c r="N29" s="145" t="n"/>
-      <c r="O29" s="145" t="inlineStr">
+      <c r="N29" s="167" t="n"/>
+      <c r="O29" s="167" t="inlineStr">
         <is>
           <t xml:space="preserve">undated </t>
         </is>
       </c>
-      <c r="P29" s="145" t="n"/>
-      <c r="Q29" s="145" t="n"/>
-      <c r="R29" s="137" t="inlineStr">
+      <c r="P29" s="167" t="n"/>
+      <c r="Q29" s="167" t="n"/>
+      <c r="R29" s="158" t="inlineStr">
         <is>
           <t xml:space="preserve">Copyright Undetermined </t>
         </is>
       </c>
-      <c r="S29" s="145" t="n"/>
-      <c r="T29" s="145" t="inlineStr">
+      <c r="S29" s="167" t="n"/>
+      <c r="T29" s="167" t="inlineStr">
         <is>
           <t>Box 5 Folder 9 Item 5</t>
         </is>
       </c>
-      <c r="U29" s="147" t="inlineStr">
+      <c r="U29" s="169" t="inlineStr">
         <is>
           <t xml:space="preserve">Glass Down, Leave in Sleeve </t>
         </is>
       </c>
-      <c r="V29" s="145" t="inlineStr">
+      <c r="V29" s="167" t="inlineStr">
         <is>
           <t>ZWU_SCA0319.B05.F09.04</t>
         </is>
       </c>
-      <c r="W29" s="149" t="n">
+      <c r="W29" s="171" t="n">
         <v>45497</v>
       </c>
-      <c r="X29" s="145" t="inlineStr">
+      <c r="X29" s="167" t="inlineStr">
         <is>
           <t>JG, SK</t>
         </is>
       </c>
-      <c r="Y29" s="141" t="inlineStr">
+      <c r="Y29" s="164" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
       </c>
-      <c r="Z29" s="145" t="inlineStr">
+      <c r="Z29" s="167" t="inlineStr">
         <is>
           <t>GH</t>
         </is>
       </c>
-      <c r="AA29" s="145" t="n"/>
-      <c r="AB29" s="145" t="n"/>
-      <c r="AC29" s="145" t="n"/>
-      <c r="AD29" s="145" t="n"/>
-      <c r="AE29" s="145" t="n"/>
+      <c r="AA29" s="167" t="n"/>
+      <c r="AB29" s="167" t="n"/>
+      <c r="AC29" s="167" t="n"/>
+      <c r="AD29" s="167" t="n"/>
+      <c r="AE29" s="167" t="n"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="143" t="inlineStr">
+      <c r="A30" s="165" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B30" s="144" t="n">
+      <c r="B30" s="166" t="n">
         <v>13250</v>
       </c>
-      <c r="C30" s="145" t="n"/>
-      <c r="D30" s="145" t="n"/>
-      <c r="E30" s="145" t="n"/>
-      <c r="F30" s="146" t="inlineStr">
+      <c r="C30" s="167" t="n"/>
+      <c r="D30" s="167" t="n"/>
+      <c r="E30" s="167" t="n"/>
+      <c r="F30" s="168" t="inlineStr">
         <is>
           <t>Induction meter documents and photographs</t>
         </is>
       </c>
-      <c r="G30" s="145" t="n"/>
-      <c r="H30" s="147" t="inlineStr">
+      <c r="G30" s="167" t="n"/>
+      <c r="H30" s="169" t="inlineStr">
         <is>
           <t>Photograph of Induction Meter, Undated  06</t>
         </is>
       </c>
-      <c r="I30" s="145" t="n"/>
-      <c r="J30" s="145" t="n"/>
-      <c r="K30" s="145" t="n"/>
-      <c r="L30" s="145" t="n"/>
-      <c r="M30" s="144" t="n">
+      <c r="I30" s="167" t="n"/>
+      <c r="J30" s="167" t="n"/>
+      <c r="K30" s="167" t="n"/>
+      <c r="L30" s="167" t="n"/>
+      <c r="M30" s="166" t="n">
         <v>1902</v>
       </c>
-      <c r="N30" s="145" t="n"/>
-      <c r="O30" s="145" t="inlineStr">
+      <c r="N30" s="167" t="n"/>
+      <c r="O30" s="167" t="inlineStr">
         <is>
           <t xml:space="preserve">undated </t>
         </is>
       </c>
-      <c r="P30" s="145" t="n"/>
-      <c r="Q30" s="145" t="n"/>
-      <c r="R30" s="137" t="inlineStr">
+      <c r="P30" s="167" t="n"/>
+      <c r="Q30" s="167" t="n"/>
+      <c r="R30" s="158" t="inlineStr">
         <is>
           <t xml:space="preserve">Copyright Undetermined </t>
         </is>
       </c>
-      <c r="S30" s="145" t="n"/>
-      <c r="T30" s="145" t="inlineStr">
+      <c r="S30" s="167" t="n"/>
+      <c r="T30" s="167" t="inlineStr">
         <is>
           <t>Box 5 Folder 9 Item 6</t>
         </is>
       </c>
-      <c r="U30" s="147" t="inlineStr">
+      <c r="U30" s="169" t="inlineStr">
         <is>
           <t xml:space="preserve">Glass Down, Leave in Sleeve </t>
         </is>
       </c>
-      <c r="V30" s="145" t="inlineStr">
+      <c r="V30" s="167" t="inlineStr">
         <is>
           <t>ZWU_SCA0319.B05.F09.05</t>
         </is>
       </c>
-      <c r="W30" s="149" t="n">
+      <c r="W30" s="171" t="n">
         <v>45497</v>
       </c>
-      <c r="X30" s="145" t="inlineStr">
+      <c r="X30" s="167" t="inlineStr">
         <is>
           <t>JG, SK</t>
         </is>
       </c>
-      <c r="Y30" s="141" t="inlineStr">
+      <c r="Y30" s="164" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
       </c>
-      <c r="Z30" s="145" t="inlineStr">
+      <c r="Z30" s="167" t="inlineStr">
         <is>
           <t>GH</t>
         </is>
       </c>
-      <c r="AA30" s="145" t="n"/>
-      <c r="AB30" s="145" t="n"/>
-      <c r="AC30" s="145" t="n"/>
-      <c r="AD30" s="145" t="n"/>
-      <c r="AE30" s="145" t="n"/>
+      <c r="AA30" s="167" t="n"/>
+      <c r="AB30" s="167" t="n"/>
+      <c r="AC30" s="167" t="n"/>
+      <c r="AD30" s="167" t="n"/>
+      <c r="AE30" s="167" t="n"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="143" t="inlineStr">
+      <c r="A31" s="165" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B31" s="144" t="n">
+      <c r="B31" s="166" t="n">
         <v>13250</v>
       </c>
-      <c r="C31" s="145" t="n"/>
-      <c r="D31" s="145" t="n"/>
-      <c r="E31" s="145" t="n"/>
-      <c r="F31" s="146" t="inlineStr">
+      <c r="C31" s="167" t="n"/>
+      <c r="D31" s="167" t="n"/>
+      <c r="E31" s="167" t="n"/>
+      <c r="F31" s="168" t="inlineStr">
         <is>
           <t>Induction meter documents and photographs</t>
         </is>
       </c>
-      <c r="G31" s="145" t="n"/>
-      <c r="H31" s="147" t="inlineStr">
+      <c r="G31" s="167" t="n"/>
+      <c r="H31" s="169" t="inlineStr">
         <is>
           <t>Photograph of Induction Meter, Undated  07</t>
         </is>
       </c>
-      <c r="I31" s="145" t="n"/>
-      <c r="J31" s="145" t="n"/>
-      <c r="K31" s="145" t="n"/>
-      <c r="L31" s="145" t="n"/>
-      <c r="M31" s="144" t="n">
+      <c r="I31" s="167" t="n"/>
+      <c r="J31" s="167" t="n"/>
+      <c r="K31" s="167" t="n"/>
+      <c r="L31" s="167" t="n"/>
+      <c r="M31" s="166" t="n">
         <v>1902</v>
       </c>
-      <c r="N31" s="145" t="n"/>
-      <c r="O31" s="145" t="inlineStr">
+      <c r="N31" s="167" t="n"/>
+      <c r="O31" s="167" t="inlineStr">
         <is>
           <t xml:space="preserve">undated </t>
         </is>
       </c>
-      <c r="P31" s="145" t="n"/>
-      <c r="Q31" s="145" t="n"/>
-      <c r="R31" s="137" t="inlineStr">
+      <c r="P31" s="167" t="n"/>
+      <c r="Q31" s="167" t="n"/>
+      <c r="R31" s="158" t="inlineStr">
         <is>
           <t xml:space="preserve">Copyright Undetermined </t>
         </is>
       </c>
-      <c r="S31" s="145" t="n"/>
-      <c r="T31" s="145" t="inlineStr">
+      <c r="S31" s="167" t="n"/>
+      <c r="T31" s="167" t="inlineStr">
         <is>
           <t>Box 5 Folder 9 Item 7</t>
         </is>
       </c>
-      <c r="U31" s="147" t="inlineStr">
+      <c r="U31" s="169" t="inlineStr">
         <is>
           <t xml:space="preserve">Glass Down, Leave in Sleeve </t>
         </is>
       </c>
-      <c r="V31" s="145" t="inlineStr">
+      <c r="V31" s="167" t="inlineStr">
         <is>
           <t>ZWU_SCA0319.B05.F09.06</t>
         </is>
       </c>
-      <c r="W31" s="149" t="n">
+      <c r="W31" s="171" t="n">
         <v>45497</v>
       </c>
-      <c r="X31" s="145" t="inlineStr">
+      <c r="X31" s="167" t="inlineStr">
         <is>
           <t>JG, SK</t>
         </is>
       </c>
-      <c r="Y31" s="141" t="inlineStr">
+      <c r="Y31" s="164" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
       </c>
-      <c r="Z31" s="145" t="inlineStr">
+      <c r="Z31" s="167" t="inlineStr">
         <is>
           <t>GH</t>
         </is>
       </c>
-      <c r="AA31" s="145" t="n"/>
-      <c r="AB31" s="145" t="n"/>
-      <c r="AC31" s="145" t="n"/>
-      <c r="AD31" s="145" t="n"/>
-      <c r="AE31" s="145" t="n"/>
+      <c r="AA31" s="167" t="n"/>
+      <c r="AB31" s="167" t="n"/>
+      <c r="AC31" s="167" t="n"/>
+      <c r="AD31" s="167" t="n"/>
+      <c r="AE31" s="167" t="n"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="143" t="inlineStr">
+      <c r="A32" s="165" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B32" s="144" t="n">
+      <c r="B32" s="166" t="n">
         <v>13250</v>
       </c>
-      <c r="C32" s="145" t="n"/>
-      <c r="D32" s="145" t="n"/>
-      <c r="E32" s="145" t="n"/>
-      <c r="F32" s="146" t="inlineStr">
+      <c r="C32" s="167" t="n"/>
+      <c r="D32" s="167" t="n"/>
+      <c r="E32" s="167" t="n"/>
+      <c r="F32" s="168" t="inlineStr">
         <is>
           <t>Induction meter documents and photographs</t>
         </is>
       </c>
-      <c r="G32" s="145" t="n"/>
-      <c r="H32" s="147" t="inlineStr">
+      <c r="G32" s="167" t="n"/>
+      <c r="H32" s="169" t="inlineStr">
         <is>
           <t>Photograph of Induction Meter, Undated  08</t>
         </is>
       </c>
-      <c r="I32" s="145" t="n"/>
-      <c r="J32" s="145" t="n"/>
-      <c r="K32" s="145" t="n"/>
-      <c r="L32" s="145" t="n"/>
-      <c r="M32" s="144" t="n">
+      <c r="I32" s="167" t="n"/>
+      <c r="J32" s="167" t="n"/>
+      <c r="K32" s="167" t="n"/>
+      <c r="L32" s="167" t="n"/>
+      <c r="M32" s="166" t="n">
         <v>1902</v>
       </c>
-      <c r="N32" s="145" t="n"/>
-      <c r="O32" s="145" t="inlineStr">
+      <c r="N32" s="167" t="n"/>
+      <c r="O32" s="167" t="inlineStr">
         <is>
           <t xml:space="preserve">undated </t>
         </is>
       </c>
-      <c r="P32" s="145" t="n"/>
-      <c r="Q32" s="145" t="n"/>
-      <c r="R32" s="137" t="inlineStr">
+      <c r="P32" s="167" t="n"/>
+      <c r="Q32" s="167" t="n"/>
+      <c r="R32" s="158" t="inlineStr">
         <is>
           <t xml:space="preserve">Copyright Undetermined </t>
         </is>
       </c>
-      <c r="S32" s="145" t="n"/>
-      <c r="T32" s="145" t="inlineStr">
+      <c r="S32" s="167" t="n"/>
+      <c r="T32" s="167" t="inlineStr">
         <is>
           <t>Box 5 Folder 9 Item 8</t>
         </is>
       </c>
-      <c r="U32" s="147" t="inlineStr">
+      <c r="U32" s="169" t="inlineStr">
         <is>
           <t xml:space="preserve">Glass Down, Leave in Sleeve </t>
         </is>
       </c>
-      <c r="V32" s="145" t="inlineStr">
+      <c r="V32" s="167" t="inlineStr">
         <is>
           <t>ZWU_SCA0319.B05.F09.07</t>
         </is>
       </c>
-      <c r="W32" s="149" t="n">
+      <c r="W32" s="171" t="n">
         <v>45497</v>
       </c>
-      <c r="X32" s="145" t="inlineStr">
+      <c r="X32" s="167" t="inlineStr">
         <is>
           <t>JG, SK</t>
         </is>
       </c>
-      <c r="Y32" s="141" t="inlineStr">
+      <c r="Y32" s="164" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
       </c>
-      <c r="Z32" s="145" t="inlineStr">
+      <c r="Z32" s="167" t="inlineStr">
         <is>
           <t>GH</t>
         </is>
       </c>
-      <c r="AA32" s="145" t="n"/>
-      <c r="AB32" s="145" t="n"/>
-      <c r="AC32" s="145" t="n"/>
-      <c r="AD32" s="145" t="n"/>
-      <c r="AE32" s="145" t="n"/>
+      <c r="AA32" s="167" t="n"/>
+      <c r="AB32" s="167" t="n"/>
+      <c r="AC32" s="167" t="n"/>
+      <c r="AD32" s="167" t="n"/>
+      <c r="AE32" s="167" t="n"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="143" t="inlineStr">
+      <c r="A33" s="165" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B33" s="144" t="n">
+      <c r="B33" s="166" t="n">
         <v>13250</v>
       </c>
-      <c r="C33" s="145" t="n"/>
-      <c r="D33" s="145" t="n"/>
-      <c r="E33" s="145" t="n"/>
-      <c r="F33" s="146" t="inlineStr">
+      <c r="C33" s="167" t="n"/>
+      <c r="D33" s="167" t="n"/>
+      <c r="E33" s="167" t="n"/>
+      <c r="F33" s="168" t="inlineStr">
         <is>
           <t>Induction meter documents and photographs</t>
         </is>
       </c>
-      <c r="G33" s="145" t="n"/>
-      <c r="H33" s="147" t="inlineStr">
+      <c r="G33" s="167" t="n"/>
+      <c r="H33" s="169" t="inlineStr">
         <is>
           <t>Photograph of Induction Meter, Undated  09</t>
         </is>
       </c>
-      <c r="I33" s="145" t="n"/>
-      <c r="J33" s="145" t="n"/>
-      <c r="K33" s="145" t="n"/>
-      <c r="L33" s="145" t="n"/>
-      <c r="M33" s="144" t="n">
+      <c r="I33" s="167" t="n"/>
+      <c r="J33" s="167" t="n"/>
+      <c r="K33" s="167" t="n"/>
+      <c r="L33" s="167" t="n"/>
+      <c r="M33" s="166" t="n">
         <v>1902</v>
       </c>
-      <c r="N33" s="145" t="n"/>
-      <c r="O33" s="145" t="inlineStr">
+      <c r="N33" s="167" t="n"/>
+      <c r="O33" s="167" t="inlineStr">
         <is>
           <t xml:space="preserve">undated </t>
         </is>
       </c>
-      <c r="P33" s="145" t="n"/>
-      <c r="Q33" s="145" t="n"/>
-      <c r="R33" s="137" t="inlineStr">
+      <c r="P33" s="167" t="n"/>
+      <c r="Q33" s="167" t="n"/>
+      <c r="R33" s="158" t="inlineStr">
         <is>
           <t xml:space="preserve">Copyright Undetermined </t>
         </is>
       </c>
-      <c r="S33" s="145" t="n"/>
-      <c r="T33" s="145" t="inlineStr">
+      <c r="S33" s="167" t="n"/>
+      <c r="T33" s="167" t="inlineStr">
         <is>
           <t>Box 5 Folder 9 Item 9</t>
         </is>
       </c>
-      <c r="U33" s="147" t="inlineStr">
+      <c r="U33" s="169" t="inlineStr">
         <is>
           <t xml:space="preserve">Glass Down, Leave in Sleeve </t>
         </is>
       </c>
-      <c r="V33" s="145" t="inlineStr">
+      <c r="V33" s="167" t="inlineStr">
         <is>
           <t>ZWU_SCA0319.B05.F09.08</t>
         </is>
       </c>
-      <c r="W33" s="149" t="n">
+      <c r="W33" s="171" t="n">
         <v>45497</v>
       </c>
-      <c r="X33" s="145" t="inlineStr">
+      <c r="X33" s="167" t="inlineStr">
         <is>
           <t>JG, SK</t>
         </is>
       </c>
-      <c r="Y33" s="141" t="inlineStr">
+      <c r="Y33" s="164" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
       </c>
-      <c r="Z33" s="145" t="inlineStr">
+      <c r="Z33" s="167" t="inlineStr">
         <is>
           <t>GH</t>
         </is>
       </c>
-      <c r="AA33" s="145" t="n"/>
-      <c r="AB33" s="145" t="n"/>
-      <c r="AC33" s="145" t="n"/>
-      <c r="AD33" s="145" t="n"/>
-      <c r="AE33" s="145" t="n"/>
+      <c r="AA33" s="167" t="n"/>
+      <c r="AB33" s="167" t="n"/>
+      <c r="AC33" s="167" t="n"/>
+      <c r="AD33" s="167" t="n"/>
+      <c r="AE33" s="167" t="n"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="143" t="inlineStr">
+      <c r="A34" s="165" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B34" s="144" t="n">
+      <c r="B34" s="166" t="n">
         <v>13250</v>
       </c>
-      <c r="C34" s="145" t="n"/>
-      <c r="D34" s="145" t="n"/>
-      <c r="E34" s="145" t="n"/>
-      <c r="F34" s="146" t="inlineStr">
+      <c r="C34" s="167" t="n"/>
+      <c r="D34" s="167" t="n"/>
+      <c r="E34" s="167" t="n"/>
+      <c r="F34" s="168" t="inlineStr">
         <is>
           <t>Induction meter documents and photographs</t>
         </is>
       </c>
-      <c r="G34" s="145" t="n"/>
-      <c r="H34" s="147" t="inlineStr">
+      <c r="G34" s="167" t="n"/>
+      <c r="H34" s="169" t="inlineStr">
         <is>
           <t>Photograph of Induction Meter, Undated  10</t>
         </is>
       </c>
-      <c r="I34" s="145" t="n"/>
-      <c r="J34" s="145" t="n"/>
-      <c r="K34" s="145" t="n"/>
-      <c r="L34" s="145" t="n"/>
-      <c r="M34" s="144" t="n">
+      <c r="I34" s="167" t="n"/>
+      <c r="J34" s="167" t="n"/>
+      <c r="K34" s="167" t="n"/>
+      <c r="L34" s="167" t="n"/>
+      <c r="M34" s="166" t="n">
         <v>1902</v>
       </c>
-      <c r="N34" s="145" t="n"/>
-      <c r="O34" s="145" t="inlineStr">
+      <c r="N34" s="167" t="n"/>
+      <c r="O34" s="167" t="inlineStr">
         <is>
           <t xml:space="preserve">undated </t>
         </is>
       </c>
-      <c r="P34" s="145" t="n"/>
-      <c r="Q34" s="145" t="n"/>
-      <c r="R34" s="137" t="inlineStr">
+      <c r="P34" s="167" t="n"/>
+      <c r="Q34" s="167" t="n"/>
+      <c r="R34" s="158" t="inlineStr">
         <is>
           <t xml:space="preserve">Copyright Undetermined </t>
         </is>
       </c>
-      <c r="S34" s="145" t="n"/>
-      <c r="T34" s="145" t="inlineStr">
+      <c r="S34" s="167" t="n"/>
+      <c r="T34" s="167" t="inlineStr">
         <is>
           <t>Box 5 Folder 9 Item 10</t>
         </is>
       </c>
-      <c r="U34" s="147" t="inlineStr">
+      <c r="U34" s="169" t="inlineStr">
         <is>
           <t xml:space="preserve">Glass Down, Leave in Sleeve </t>
         </is>
       </c>
-      <c r="V34" s="145" t="inlineStr">
+      <c r="V34" s="167" t="inlineStr">
         <is>
           <t>ZWU_SCA0319.B05.F09.09</t>
         </is>
       </c>
-      <c r="W34" s="149" t="n">
+      <c r="W34" s="171" t="n">
         <v>45497</v>
       </c>
-      <c r="X34" s="145" t="inlineStr">
+      <c r="X34" s="167" t="inlineStr">
         <is>
           <t>JG, SK</t>
         </is>
       </c>
-      <c r="Y34" s="141" t="inlineStr">
+      <c r="Y34" s="164" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
       </c>
-      <c r="Z34" s="145" t="inlineStr">
+      <c r="Z34" s="167" t="inlineStr">
         <is>
           <t>GH</t>
         </is>
       </c>
-      <c r="AA34" s="145" t="n"/>
-      <c r="AB34" s="145" t="n"/>
-      <c r="AC34" s="145" t="n"/>
-      <c r="AD34" s="145" t="n"/>
-      <c r="AE34" s="145" t="n"/>
+      <c r="AA34" s="167" t="n"/>
+      <c r="AB34" s="167" t="n"/>
+      <c r="AC34" s="167" t="n"/>
+      <c r="AD34" s="167" t="n"/>
+      <c r="AE34" s="167" t="n"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="114" t="inlineStr">
@@ -22589,95 +22671,95 @@
       <c r="AE35" s="68" t="n"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="143" t="inlineStr">
+      <c r="A36" s="165" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B36" s="144" t="n">
+      <c r="B36" s="166" t="n">
         <v>13250</v>
       </c>
-      <c r="C36" s="145" t="n"/>
-      <c r="D36" s="145" t="n"/>
-      <c r="E36" s="145" t="n"/>
-      <c r="F36" s="146" t="inlineStr">
+      <c r="C36" s="167" t="n"/>
+      <c r="D36" s="167" t="n"/>
+      <c r="E36" s="167" t="n"/>
+      <c r="F36" s="168" t="inlineStr">
         <is>
           <t>Induction meter documents and photographs</t>
         </is>
       </c>
-      <c r="G36" s="145" t="n"/>
-      <c r="H36" s="145" t="inlineStr">
+      <c r="G36" s="167" t="n"/>
+      <c r="H36" s="167" t="inlineStr">
         <is>
           <t xml:space="preserve">Enclosure From Marks &amp; Clerk, London, to W. Stanley Esq. </t>
         </is>
       </c>
-      <c r="I36" s="145" t="inlineStr">
+      <c r="I36" s="167" t="inlineStr">
         <is>
           <t>Marks &amp; Clerk (London)</t>
         </is>
       </c>
-      <c r="J36" s="145" t="n"/>
-      <c r="K36" s="145" t="n"/>
-      <c r="L36" s="145" t="n"/>
-      <c r="M36" s="144" t="n">
+      <c r="J36" s="167" t="n"/>
+      <c r="K36" s="167" t="n"/>
+      <c r="L36" s="167" t="n"/>
+      <c r="M36" s="166" t="n">
         <v>1902</v>
       </c>
-      <c r="N36" s="145" t="n"/>
-      <c r="O36" s="145" t="inlineStr">
+      <c r="N36" s="167" t="n"/>
+      <c r="O36" s="167" t="inlineStr">
         <is>
           <t xml:space="preserve">undated </t>
         </is>
       </c>
-      <c r="P36" s="145" t="n"/>
-      <c r="Q36" s="145" t="n"/>
-      <c r="R36" s="137" t="inlineStr">
+      <c r="P36" s="167" t="n"/>
+      <c r="Q36" s="167" t="n"/>
+      <c r="R36" s="158" t="inlineStr">
         <is>
           <t xml:space="preserve">Copyright Undetermined </t>
         </is>
       </c>
-      <c r="S36" s="145" t="n"/>
-      <c r="T36" s="145" t="inlineStr">
+      <c r="S36" s="167" t="n"/>
+      <c r="T36" s="167" t="inlineStr">
         <is>
           <t>Box 5 Folder 9 Item 12</t>
         </is>
       </c>
-      <c r="U36" s="145" t="inlineStr">
+      <c r="U36" s="167" t="inlineStr">
         <is>
           <t>Glass down, leave in sleeve.</t>
         </is>
       </c>
-      <c r="V36" s="145" t="inlineStr">
+      <c r="V36" s="167" t="inlineStr">
         <is>
           <t>ZWU_SCA0319.B05.F09.11</t>
         </is>
       </c>
-      <c r="W36" s="149" t="n">
+      <c r="W36" s="171" t="n">
         <v>45497</v>
       </c>
-      <c r="X36" s="145" t="inlineStr">
+      <c r="X36" s="167" t="inlineStr">
         <is>
           <t>JG, SK</t>
         </is>
       </c>
-      <c r="Y36" s="141" t="inlineStr">
+      <c r="Y36" s="164" t="inlineStr">
         <is>
           <t>Fail</t>
         </is>
       </c>
-      <c r="Z36" s="145" t="inlineStr">
+      <c r="Z36" s="167" t="inlineStr">
         <is>
           <t>GH</t>
         </is>
       </c>
-      <c r="AA36" s="145" t="inlineStr">
+      <c r="AA36" s="167" t="inlineStr">
         <is>
           <t>Can delete the second page as there isn't any information on it</t>
         </is>
       </c>
-      <c r="AB36" s="145" t="n"/>
-      <c r="AC36" s="145" t="n"/>
-      <c r="AD36" s="145" t="n"/>
-      <c r="AE36" s="145" t="n"/>
+      <c r="AB36" s="167" t="n"/>
+      <c r="AC36" s="167" t="n"/>
+      <c r="AD36" s="167" t="n"/>
+      <c r="AE36" s="167" t="n"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="114" t="inlineStr">
@@ -34490,95 +34572,95 @@
       <c r="AD1" s="112" t="n"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="143" t="inlineStr">
+      <c r="A2" s="165" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B2" s="144" t="n">
+      <c r="B2" s="166" t="n">
         <v>13269</v>
       </c>
-      <c r="C2" s="145" t="n"/>
-      <c r="D2" s="145" t="n"/>
-      <c r="E2" s="145" t="n"/>
-      <c r="F2" s="143" t="inlineStr">
+      <c r="C2" s="167" t="n"/>
+      <c r="D2" s="167" t="n"/>
+      <c r="E2" s="167" t="n"/>
+      <c r="F2" s="165" t="inlineStr">
         <is>
           <t>General Incandescent Arc Light Company Bulletins</t>
         </is>
       </c>
-      <c r="G2" s="145" t="n"/>
-      <c r="H2" s="143" t="inlineStr">
+      <c r="G2" s="167" t="n"/>
+      <c r="H2" s="165" t="inlineStr">
         <is>
           <t>General Incandescent Arc Light Company Send for G.I Bulletins</t>
         </is>
       </c>
-      <c r="I2" s="145" t="n"/>
-      <c r="J2" s="146" t="inlineStr">
+      <c r="I2" s="167" t="n"/>
+      <c r="J2" s="168" t="inlineStr">
         <is>
           <t>General Incandescent Light Company (New York, NY)</t>
         </is>
       </c>
-      <c r="K2" s="145" t="n"/>
-      <c r="L2" s="145" t="n"/>
-      <c r="M2" s="143" t="inlineStr">
+      <c r="K2" s="167" t="n"/>
+      <c r="L2" s="167" t="n"/>
+      <c r="M2" s="165" t="inlineStr">
         <is>
           <t>1903-1905</t>
         </is>
       </c>
-      <c r="N2" s="145" t="n"/>
-      <c r="O2" s="146" t="inlineStr">
+      <c r="N2" s="167" t="n"/>
+      <c r="O2" s="168" t="inlineStr">
         <is>
           <t>Press of Cowan &amp; Ditmars, New York</t>
         </is>
       </c>
-      <c r="P2" s="143" t="inlineStr">
+      <c r="P2" s="165" t="inlineStr">
         <is>
           <t>1903-1904</t>
         </is>
       </c>
-      <c r="Q2" s="145" t="n"/>
-      <c r="R2" s="145" t="n"/>
-      <c r="S2" s="143" t="inlineStr">
+      <c r="Q2" s="167" t="n"/>
+      <c r="R2" s="167" t="n"/>
+      <c r="S2" s="165" t="inlineStr">
         <is>
           <t xml:space="preserve">No Copyright - United States </t>
         </is>
       </c>
-      <c r="T2" s="145" t="n"/>
-      <c r="U2" s="147" t="inlineStr">
+      <c r="T2" s="167" t="n"/>
+      <c r="U2" s="169" t="inlineStr">
         <is>
           <t xml:space="preserve">Box 6, Folder 1, Item 1 </t>
         </is>
       </c>
-      <c r="V2" s="147" t="inlineStr">
+      <c r="V2" s="169" t="inlineStr">
         <is>
           <t xml:space="preserve">Glass up. Duplicates, Scan Only First Copy on Right with "Missing #335" written on the right side margin. </t>
         </is>
       </c>
-      <c r="W2" s="143" t="inlineStr">
+      <c r="W2" s="165" t="inlineStr">
         <is>
           <t>ZWU_SCA0319.B06.F01.p01</t>
         </is>
       </c>
-      <c r="X2" s="152" t="n">
+      <c r="X2" s="172" t="n">
         <v>45492</v>
       </c>
-      <c r="Y2" s="145" t="inlineStr">
+      <c r="Y2" s="167" t="inlineStr">
         <is>
           <t xml:space="preserve">JG, SK </t>
         </is>
       </c>
-      <c r="Z2" s="145" t="n"/>
-      <c r="AA2" s="141" t="n"/>
-      <c r="AB2" s="141" t="n"/>
-      <c r="AC2" s="141" t="n"/>
-      <c r="AD2" s="153" t="inlineStr">
+      <c r="Z2" s="167" t="n"/>
+      <c r="AA2" s="164" t="n"/>
+      <c r="AB2" s="164" t="n"/>
+      <c r="AC2" s="164" t="n"/>
+      <c r="AD2" s="173" t="inlineStr">
         <is>
           <t>Found multiple copies of the same piece just marked up slightly differently</t>
         </is>
       </c>
-      <c r="AE2" s="141" t="n"/>
-      <c r="AF2" s="141" t="n"/>
-      <c r="AG2" s="141" t="n"/>
+      <c r="AE2" s="164" t="n"/>
+      <c r="AF2" s="164" t="n"/>
+      <c r="AG2" s="164" t="n"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="114" t="inlineStr">
@@ -38549,89 +38631,89 @@
       <c r="AG51" s="139" t="n"/>
     </row>
     <row r="52" ht="90" customHeight="1">
-      <c r="A52" s="143" t="inlineStr">
+      <c r="A52" s="165" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B52" s="144" t="n">
+      <c r="B52" s="166" t="n">
         <v>13269</v>
       </c>
-      <c r="C52" s="145" t="n"/>
-      <c r="D52" s="145" t="n"/>
-      <c r="E52" s="145" t="n"/>
-      <c r="F52" s="143" t="inlineStr">
+      <c r="C52" s="167" t="n"/>
+      <c r="D52" s="167" t="n"/>
+      <c r="E52" s="167" t="n"/>
+      <c r="F52" s="165" t="inlineStr">
         <is>
           <t>General Incandescent Arc Light Company Bulletins</t>
         </is>
       </c>
-      <c r="G52" s="145" t="n"/>
-      <c r="H52" s="143" t="inlineStr">
+      <c r="G52" s="167" t="n"/>
+      <c r="H52" s="165" t="inlineStr">
         <is>
           <t>General Incandescent Arc Light Co. Bulletin No. 174</t>
         </is>
       </c>
-      <c r="I52" s="143" t="inlineStr">
+      <c r="I52" s="165" t="inlineStr">
         <is>
           <t xml:space="preserve">Titile transcribed from bulletin </t>
         </is>
       </c>
-      <c r="J52" s="146" t="inlineStr">
+      <c r="J52" s="168" t="inlineStr">
         <is>
           <t>General Incandescent Light Company (New York, NY)</t>
         </is>
       </c>
-      <c r="K52" s="145" t="n"/>
-      <c r="L52" s="145" t="n"/>
-      <c r="M52" s="143" t="inlineStr">
+      <c r="K52" s="167" t="n"/>
+      <c r="L52" s="167" t="n"/>
+      <c r="M52" s="165" t="inlineStr">
         <is>
           <t>1903-1905</t>
         </is>
       </c>
-      <c r="N52" s="145" t="n"/>
-      <c r="O52" s="145" t="n"/>
-      <c r="P52" s="145" t="n"/>
-      <c r="Q52" s="154" t="n">
+      <c r="N52" s="167" t="n"/>
+      <c r="O52" s="167" t="n"/>
+      <c r="P52" s="167" t="n"/>
+      <c r="Q52" s="174" t="n">
         <v>1248</v>
       </c>
-      <c r="R52" s="145" t="n"/>
-      <c r="S52" s="143" t="inlineStr">
+      <c r="R52" s="167" t="n"/>
+      <c r="S52" s="165" t="inlineStr">
         <is>
           <t xml:space="preserve">No Copyright - United States </t>
         </is>
       </c>
-      <c r="T52" s="145" t="n"/>
-      <c r="U52" s="147" t="inlineStr">
+      <c r="T52" s="167" t="n"/>
+      <c r="U52" s="169" t="inlineStr">
         <is>
           <t>Box 6, Folder 2, Bulletin 2174</t>
         </is>
       </c>
-      <c r="V52" s="146" t="inlineStr">
+      <c r="V52" s="168" t="inlineStr">
         <is>
           <t xml:space="preserve">Scan each bulletin as it's own file, glass down. </t>
         </is>
       </c>
-      <c r="W52" s="143" t="inlineStr">
+      <c r="W52" s="165" t="inlineStr">
         <is>
           <t>ZWU_SCA0319.B06.F02.Bull.174</t>
         </is>
       </c>
-      <c r="X52" s="152" t="n">
+      <c r="X52" s="172" t="n">
         <v>45495</v>
       </c>
-      <c r="Y52" s="145" t="inlineStr">
+      <c r="Y52" s="167" t="inlineStr">
         <is>
           <t>MC, SK</t>
         </is>
       </c>
-      <c r="Z52" s="145" t="n"/>
-      <c r="AA52" s="139" t="n"/>
-      <c r="AB52" s="141" t="n"/>
-      <c r="AC52" s="139" t="n"/>
-      <c r="AD52" s="153" t="n"/>
-      <c r="AE52" s="139" t="n"/>
-      <c r="AF52" s="139" t="n"/>
-      <c r="AG52" s="139" t="n"/>
+      <c r="Z52" s="167" t="n"/>
+      <c r="AA52" s="160" t="n"/>
+      <c r="AB52" s="164" t="n"/>
+      <c r="AC52" s="160" t="n"/>
+      <c r="AD52" s="173" t="n"/>
+      <c r="AE52" s="160" t="n"/>
+      <c r="AF52" s="160" t="n"/>
+      <c r="AG52" s="160" t="n"/>
     </row>
     <row r="53" ht="90" customHeight="1">
       <c r="A53" s="114" t="inlineStr">
@@ -39194,84 +39276,89 @@
       <c r="AD59" s="112" t="n"/>
     </row>
     <row r="60" ht="90" customHeight="1">
-      <c r="A60" s="114" t="inlineStr">
+      <c r="A60" s="175" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B60" s="31" t="n">
+      <c r="B60" s="176" t="n">
         <v>13269</v>
       </c>
-      <c r="C60" s="68" t="n"/>
-      <c r="D60" s="68" t="n"/>
-      <c r="E60" s="68" t="n"/>
-      <c r="F60" s="114" t="inlineStr">
+      <c r="C60" s="177" t="n"/>
+      <c r="D60" s="177" t="n"/>
+      <c r="E60" s="177" t="n"/>
+      <c r="F60" s="175" t="inlineStr">
         <is>
           <t>General Incandescent Arc Light Company Bulletins</t>
         </is>
       </c>
-      <c r="G60" s="68" t="n"/>
-      <c r="H60" s="114" t="inlineStr">
+      <c r="G60" s="177" t="n"/>
+      <c r="H60" s="175" t="inlineStr">
         <is>
           <t>General Incandescent Arc Light Co. Bulletin No. 340</t>
         </is>
       </c>
-      <c r="I60" s="114" t="inlineStr">
+      <c r="I60" s="175" t="inlineStr">
         <is>
           <t xml:space="preserve">Titile transcribed from bulletin </t>
         </is>
       </c>
-      <c r="J60" s="22" t="inlineStr">
+      <c r="J60" s="178" t="inlineStr">
         <is>
           <t>General Incandescent Light Company (New York, NY)</t>
         </is>
       </c>
-      <c r="K60" s="68" t="n"/>
-      <c r="L60" s="68" t="n"/>
-      <c r="M60" s="114" t="inlineStr">
+      <c r="K60" s="177" t="n"/>
+      <c r="L60" s="177" t="n"/>
+      <c r="M60" s="175" t="inlineStr">
         <is>
           <t>1903-1905</t>
         </is>
       </c>
-      <c r="N60" s="68" t="n"/>
-      <c r="O60" s="68" t="n"/>
-      <c r="P60" s="68" t="n"/>
-      <c r="Q60" s="115" t="n">
+      <c r="N60" s="177" t="n"/>
+      <c r="O60" s="177" t="n"/>
+      <c r="P60" s="177" t="n"/>
+      <c r="Q60" s="179" t="n">
         <v>1462</v>
       </c>
-      <c r="R60" s="68" t="n"/>
-      <c r="S60" s="114" t="inlineStr">
+      <c r="R60" s="177" t="n"/>
+      <c r="S60" s="175" t="inlineStr">
         <is>
           <t xml:space="preserve">No Copyright - United States </t>
         </is>
       </c>
-      <c r="T60" s="68" t="n"/>
-      <c r="U60" s="77" t="inlineStr">
+      <c r="T60" s="177" t="n"/>
+      <c r="U60" s="180" t="inlineStr">
         <is>
           <t>Box 6, Folder 2, Bulletin 340</t>
         </is>
       </c>
-      <c r="V60" s="22" t="inlineStr">
+      <c r="V60" s="178" t="inlineStr">
         <is>
           <t xml:space="preserve">Scan each bulletin as it's own file, glass down. </t>
         </is>
       </c>
-      <c r="W60" s="114" t="inlineStr">
+      <c r="W60" s="175" t="inlineStr">
         <is>
           <t>ZWU_SCA0319.B06.F02.Bull.340</t>
         </is>
       </c>
-      <c r="X60" s="76" t="n">
+      <c r="X60" s="181" t="n">
         <v>45495</v>
       </c>
-      <c r="Y60" s="68" t="inlineStr">
+      <c r="Y60" s="177" t="inlineStr">
         <is>
           <t>MC, SK</t>
         </is>
       </c>
-      <c r="Z60" s="68" t="n"/>
-      <c r="AB60" s="99" t="n"/>
-      <c r="AD60" s="112" t="n"/>
+      <c r="Z60" s="177" t="n"/>
+      <c r="AA60" s="182" t="n"/>
+      <c r="AB60" s="183" t="n"/>
+      <c r="AC60" s="182" t="n"/>
+      <c r="AD60" s="184" t="n"/>
+      <c r="AE60" s="182" t="n"/>
+      <c r="AF60" s="182" t="n"/>
+      <c r="AG60" s="182" t="n"/>
     </row>
     <row r="61" ht="90" customHeight="1">
       <c r="A61" s="114" t="inlineStr">
@@ -39354,89 +39441,89 @@
       <c r="AD61" s="112" t="n"/>
     </row>
     <row r="62" ht="90" customHeight="1">
-      <c r="A62" s="143" t="inlineStr">
+      <c r="A62" s="165" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B62" s="144" t="n">
+      <c r="B62" s="166" t="n">
         <v>13269</v>
       </c>
-      <c r="C62" s="145" t="n"/>
-      <c r="D62" s="145" t="n"/>
-      <c r="E62" s="145" t="n"/>
-      <c r="F62" s="143" t="inlineStr">
+      <c r="C62" s="167" t="n"/>
+      <c r="D62" s="167" t="n"/>
+      <c r="E62" s="167" t="n"/>
+      <c r="F62" s="165" t="inlineStr">
         <is>
           <t>General Incandescent Arc Light Company Bulletins</t>
         </is>
       </c>
-      <c r="G62" s="145" t="n"/>
-      <c r="H62" s="143" t="inlineStr">
+      <c r="G62" s="167" t="n"/>
+      <c r="H62" s="165" t="inlineStr">
         <is>
           <t>General Incandescent Arc Light Co. Sheet No. 166</t>
         </is>
       </c>
-      <c r="I62" s="143" t="inlineStr">
+      <c r="I62" s="165" t="inlineStr">
         <is>
           <t xml:space="preserve">Titile transcribed from bulletin </t>
         </is>
       </c>
-      <c r="J62" s="146" t="inlineStr">
+      <c r="J62" s="168" t="inlineStr">
         <is>
           <t>General Incandescent Light Company (New York, NY)</t>
         </is>
       </c>
-      <c r="K62" s="145" t="n"/>
-      <c r="L62" s="145" t="n"/>
-      <c r="M62" s="143" t="inlineStr">
+      <c r="K62" s="167" t="n"/>
+      <c r="L62" s="167" t="n"/>
+      <c r="M62" s="165" t="inlineStr">
         <is>
           <t>1903-1905</t>
         </is>
       </c>
-      <c r="N62" s="145" t="n"/>
-      <c r="O62" s="145" t="n"/>
-      <c r="P62" s="145" t="n"/>
-      <c r="Q62" s="154" t="n">
+      <c r="N62" s="167" t="n"/>
+      <c r="O62" s="167" t="n"/>
+      <c r="P62" s="167" t="n"/>
+      <c r="Q62" s="174" t="n">
         <v>1522</v>
       </c>
-      <c r="R62" s="145" t="n"/>
-      <c r="S62" s="143" t="inlineStr">
+      <c r="R62" s="167" t="n"/>
+      <c r="S62" s="165" t="inlineStr">
         <is>
           <t xml:space="preserve">No Copyright - United States </t>
         </is>
       </c>
-      <c r="T62" s="145" t="n"/>
-      <c r="U62" s="147" t="inlineStr">
+      <c r="T62" s="167" t="n"/>
+      <c r="U62" s="169" t="inlineStr">
         <is>
           <t>Box 6, Folder 2, Sheet 166</t>
         </is>
       </c>
-      <c r="V62" s="146" t="inlineStr">
+      <c r="V62" s="168" t="inlineStr">
         <is>
           <t xml:space="preserve">Scan each bulletin as it's own file, glass down. </t>
         </is>
       </c>
-      <c r="W62" s="143" t="inlineStr">
+      <c r="W62" s="165" t="inlineStr">
         <is>
           <t>ZWU_SCA0319.B06.F02.Bull.166</t>
         </is>
       </c>
-      <c r="X62" s="152" t="n">
+      <c r="X62" s="172" t="n">
         <v>45495</v>
       </c>
-      <c r="Y62" s="145" t="inlineStr">
+      <c r="Y62" s="167" t="inlineStr">
         <is>
           <t>MC, SK</t>
         </is>
       </c>
-      <c r="Z62" s="145" t="n"/>
-      <c r="AA62" s="139" t="n"/>
-      <c r="AB62" s="141" t="n"/>
-      <c r="AC62" s="139" t="n"/>
-      <c r="AD62" s="153" t="n"/>
-      <c r="AE62" s="139" t="n"/>
-      <c r="AF62" s="139" t="n"/>
-      <c r="AG62" s="139" t="n"/>
+      <c r="Z62" s="167" t="n"/>
+      <c r="AA62" s="160" t="n"/>
+      <c r="AB62" s="164" t="n"/>
+      <c r="AC62" s="160" t="n"/>
+      <c r="AD62" s="173" t="n"/>
+      <c r="AE62" s="160" t="n"/>
+      <c r="AF62" s="160" t="n"/>
+      <c r="AG62" s="160" t="n"/>
     </row>
     <row r="63" ht="90" customHeight="1">
       <c r="A63" s="114" t="inlineStr">
@@ -40004,84 +40091,89 @@
       <c r="AD69" s="112" t="n"/>
     </row>
     <row r="70" ht="90" customHeight="1">
-      <c r="A70" s="114" t="inlineStr">
+      <c r="A70" s="175" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B70" s="31" t="n">
+      <c r="B70" s="176" t="n">
         <v>13269</v>
       </c>
-      <c r="C70" s="68" t="n"/>
-      <c r="D70" s="68" t="n"/>
-      <c r="E70" s="68" t="n"/>
-      <c r="F70" s="114" t="inlineStr">
+      <c r="C70" s="177" t="n"/>
+      <c r="D70" s="177" t="n"/>
+      <c r="E70" s="177" t="n"/>
+      <c r="F70" s="175" t="inlineStr">
         <is>
           <t>General Incandescent Arc Light Company Bulletins</t>
         </is>
       </c>
-      <c r="G70" s="68" t="n"/>
-      <c r="H70" s="114" t="inlineStr">
+      <c r="G70" s="177" t="n"/>
+      <c r="H70" s="175" t="inlineStr">
         <is>
           <t>General Incandescent Arc Light Co. Bulletin No. 340</t>
         </is>
       </c>
-      <c r="I70" s="114" t="inlineStr">
+      <c r="I70" s="175" t="inlineStr">
         <is>
           <t xml:space="preserve">Titile transcribed from bulletin </t>
         </is>
       </c>
-      <c r="J70" s="22" t="inlineStr">
+      <c r="J70" s="178" t="inlineStr">
         <is>
           <t>General Incandescent Light Company (New York, NY)</t>
         </is>
       </c>
-      <c r="K70" s="68" t="n"/>
-      <c r="L70" s="68" t="n"/>
-      <c r="M70" s="114" t="inlineStr">
+      <c r="K70" s="177" t="n"/>
+      <c r="L70" s="177" t="n"/>
+      <c r="M70" s="175" t="inlineStr">
         <is>
           <t>1903-1905</t>
         </is>
       </c>
-      <c r="N70" s="68" t="n"/>
-      <c r="O70" s="68" t="n"/>
-      <c r="P70" s="68" t="n"/>
-      <c r="Q70" s="115" t="n">
+      <c r="N70" s="177" t="n"/>
+      <c r="O70" s="177" t="n"/>
+      <c r="P70" s="177" t="n"/>
+      <c r="Q70" s="179" t="n">
         <v>1706</v>
       </c>
-      <c r="R70" s="68" t="n"/>
-      <c r="S70" s="114" t="inlineStr">
+      <c r="R70" s="177" t="n"/>
+      <c r="S70" s="175" t="inlineStr">
         <is>
           <t xml:space="preserve">No Copyright - United States </t>
         </is>
       </c>
-      <c r="T70" s="68" t="n"/>
-      <c r="U70" s="77" t="inlineStr">
+      <c r="T70" s="177" t="n"/>
+      <c r="U70" s="180" t="inlineStr">
         <is>
           <t>Box 6, Folder 2, Bulletin 340</t>
         </is>
       </c>
-      <c r="V70" s="22" t="inlineStr">
+      <c r="V70" s="178" t="inlineStr">
         <is>
           <t xml:space="preserve">Scan each bulletin as it's own file, glass down. </t>
         </is>
       </c>
-      <c r="W70" s="114" t="inlineStr">
+      <c r="W70" s="175" t="inlineStr">
         <is>
           <t>ZWU_SCA0319.B06.F02.Bull.340</t>
         </is>
       </c>
-      <c r="X70" s="76" t="n">
+      <c r="X70" s="181" t="n">
         <v>45495</v>
       </c>
-      <c r="Y70" s="68" t="inlineStr">
+      <c r="Y70" s="177" t="inlineStr">
         <is>
           <t>MC, SK</t>
         </is>
       </c>
-      <c r="Z70" s="68" t="n"/>
-      <c r="AB70" s="99" t="n"/>
-      <c r="AD70" s="112" t="n"/>
+      <c r="Z70" s="177" t="n"/>
+      <c r="AA70" s="182" t="n"/>
+      <c r="AB70" s="183" t="n"/>
+      <c r="AC70" s="182" t="n"/>
+      <c r="AD70" s="184" t="n"/>
+      <c r="AE70" s="182" t="n"/>
+      <c r="AF70" s="182" t="n"/>
+      <c r="AG70" s="182" t="n"/>
     </row>
     <row r="71" ht="90" customHeight="1">
       <c r="A71" s="143" t="inlineStr">
@@ -41222,89 +41314,89 @@
       <c r="AD84" s="112" t="n"/>
     </row>
     <row r="85" ht="90" customHeight="1">
-      <c r="A85" s="143" t="inlineStr">
+      <c r="A85" s="165" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B85" s="144" t="n">
+      <c r="B85" s="166" t="n">
         <v>13269</v>
       </c>
-      <c r="C85" s="145" t="n"/>
-      <c r="D85" s="145" t="n"/>
-      <c r="E85" s="145" t="n"/>
-      <c r="F85" s="143" t="inlineStr">
+      <c r="C85" s="167" t="n"/>
+      <c r="D85" s="167" t="n"/>
+      <c r="E85" s="167" t="n"/>
+      <c r="F85" s="165" t="inlineStr">
         <is>
           <t>General Incandescent Arc Light Company Bulletins</t>
         </is>
       </c>
-      <c r="G85" s="145" t="n"/>
-      <c r="H85" s="143" t="inlineStr">
+      <c r="G85" s="167" t="n"/>
+      <c r="H85" s="165" t="inlineStr">
         <is>
           <t>General Incandescent Arc Light Co. Bulletin No. 282</t>
         </is>
       </c>
-      <c r="I85" s="143" t="inlineStr">
+      <c r="I85" s="165" t="inlineStr">
         <is>
           <t xml:space="preserve">Titile transcribed from bulletin </t>
         </is>
       </c>
-      <c r="J85" s="146" t="inlineStr">
+      <c r="J85" s="168" t="inlineStr">
         <is>
           <t>General Incandescent Light Company (New York, NY)</t>
         </is>
       </c>
-      <c r="K85" s="145" t="n"/>
-      <c r="L85" s="145" t="n"/>
-      <c r="M85" s="143" t="inlineStr">
+      <c r="K85" s="167" t="n"/>
+      <c r="L85" s="167" t="n"/>
+      <c r="M85" s="165" t="inlineStr">
         <is>
           <t>1903-1905</t>
         </is>
       </c>
-      <c r="N85" s="145" t="n"/>
-      <c r="O85" s="145" t="n"/>
-      <c r="P85" s="145" t="n"/>
-      <c r="Q85" s="154" t="n">
+      <c r="N85" s="167" t="n"/>
+      <c r="O85" s="167" t="n"/>
+      <c r="P85" s="167" t="n"/>
+      <c r="Q85" s="174" t="n">
         <v>1887</v>
       </c>
-      <c r="R85" s="145" t="n"/>
-      <c r="S85" s="143" t="inlineStr">
+      <c r="R85" s="167" t="n"/>
+      <c r="S85" s="165" t="inlineStr">
         <is>
           <t xml:space="preserve">No Copyright - United States </t>
         </is>
       </c>
-      <c r="T85" s="145" t="n"/>
-      <c r="U85" s="147" t="inlineStr">
+      <c r="T85" s="167" t="n"/>
+      <c r="U85" s="169" t="inlineStr">
         <is>
           <t>Box 6, Folder 2, Bulletin 282</t>
         </is>
       </c>
-      <c r="V85" s="146" t="inlineStr">
+      <c r="V85" s="168" t="inlineStr">
         <is>
           <t xml:space="preserve">Scan each bulletin as it's own file, glass down. </t>
         </is>
       </c>
-      <c r="W85" s="143" t="inlineStr">
+      <c r="W85" s="165" t="inlineStr">
         <is>
           <t>ZWU_SCA0319.B06.F02.Bull.28</t>
         </is>
       </c>
-      <c r="X85" s="152" t="n">
+      <c r="X85" s="172" t="n">
         <v>45495</v>
       </c>
-      <c r="Y85" s="145" t="inlineStr">
+      <c r="Y85" s="167" t="inlineStr">
         <is>
           <t>JG</t>
         </is>
       </c>
-      <c r="Z85" s="145" t="n"/>
-      <c r="AA85" s="139" t="n"/>
-      <c r="AB85" s="141" t="n"/>
-      <c r="AC85" s="139" t="n"/>
-      <c r="AD85" s="153" t="n"/>
-      <c r="AE85" s="139" t="n"/>
-      <c r="AF85" s="139" t="n"/>
-      <c r="AG85" s="139" t="n"/>
+      <c r="Z85" s="167" t="n"/>
+      <c r="AA85" s="160" t="n"/>
+      <c r="AB85" s="164" t="n"/>
+      <c r="AC85" s="160" t="n"/>
+      <c r="AD85" s="173" t="n"/>
+      <c r="AE85" s="160" t="n"/>
+      <c r="AF85" s="160" t="n"/>
+      <c r="AG85" s="160" t="n"/>
     </row>
     <row r="86" ht="90" customHeight="1">
       <c r="A86" s="114" t="inlineStr">
@@ -49393,88 +49485,88 @@
       <c r="AF39" s="68" t="n"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="143" t="inlineStr">
+      <c r="A40" s="165" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B40" s="144" t="n">
+      <c r="B40" s="166" t="n">
         <v>13278</v>
       </c>
-      <c r="C40" s="145" t="n"/>
-      <c r="D40" s="145" t="n"/>
-      <c r="E40" s="145" t="n"/>
-      <c r="F40" s="143" t="inlineStr">
+      <c r="C40" s="167" t="n"/>
+      <c r="D40" s="167" t="n"/>
+      <c r="E40" s="167" t="n"/>
+      <c r="F40" s="165" t="inlineStr">
         <is>
           <t>Stanley patents</t>
         </is>
       </c>
-      <c r="G40" s="145" t="n"/>
-      <c r="H40" s="147" t="inlineStr">
+      <c r="G40" s="167" t="n"/>
+      <c r="H40" s="169" t="inlineStr">
         <is>
           <t>Letter from Pennie, Davis, and Goldsborough to William Stanley Jr., September 23, 1911</t>
         </is>
       </c>
-      <c r="I40" s="145" t="n"/>
-      <c r="J40" s="145" t="n"/>
-      <c r="K40" s="145" t="n"/>
-      <c r="L40" s="145" t="n"/>
-      <c r="M40" s="143" t="inlineStr">
+      <c r="I40" s="167" t="n"/>
+      <c r="J40" s="167" t="n"/>
+      <c r="K40" s="167" t="n"/>
+      <c r="L40" s="167" t="n"/>
+      <c r="M40" s="165" t="inlineStr">
         <is>
           <t>1902-1907</t>
         </is>
       </c>
-      <c r="N40" s="145" t="n"/>
-      <c r="O40" s="145" t="n"/>
-      <c r="P40" s="145" t="n"/>
-      <c r="Q40" s="156" t="n">
+      <c r="N40" s="167" t="n"/>
+      <c r="O40" s="167" t="n"/>
+      <c r="P40" s="167" t="n"/>
+      <c r="Q40" s="185" t="n">
         <v>4284</v>
       </c>
-      <c r="R40" s="145" t="n"/>
-      <c r="S40" s="143" t="inlineStr">
+      <c r="R40" s="167" t="n"/>
+      <c r="S40" s="165" t="inlineStr">
         <is>
           <t xml:space="preserve">No Copyright - United States </t>
         </is>
       </c>
-      <c r="T40" s="145" t="n"/>
-      <c r="U40" s="145" t="inlineStr">
+      <c r="T40" s="167" t="n"/>
+      <c r="U40" s="167" t="inlineStr">
         <is>
           <t>Box 7, Folder 2, Item 25</t>
         </is>
       </c>
-      <c r="V40" s="145" t="inlineStr">
+      <c r="V40" s="167" t="inlineStr">
         <is>
           <t xml:space="preserve">Glass Down. Leave in Sleeve. </t>
         </is>
       </c>
-      <c r="W40" s="145" t="inlineStr">
+      <c r="W40" s="167" t="inlineStr">
         <is>
           <t>ZWU_SCA0319.B07.F02.24.14</t>
         </is>
       </c>
-      <c r="X40" s="152" t="n">
+      <c r="X40" s="172" t="n">
         <v>45503</v>
       </c>
-      <c r="Y40" s="145" t="inlineStr">
+      <c r="Y40" s="167" t="inlineStr">
         <is>
           <t>MC</t>
         </is>
       </c>
-      <c r="Z40" s="145" t="n"/>
-      <c r="AA40" s="145" t="n"/>
-      <c r="AB40" s="145" t="inlineStr">
+      <c r="Z40" s="167" t="n"/>
+      <c r="AA40" s="167" t="n"/>
+      <c r="AB40" s="167" t="inlineStr">
         <is>
           <t>SK</t>
         </is>
       </c>
-      <c r="AC40" s="141" t="inlineStr">
+      <c r="AC40" s="164" t="inlineStr">
         <is>
           <t>Pass</t>
         </is>
       </c>
-      <c r="AD40" s="145" t="n"/>
-      <c r="AE40" s="145" t="n"/>
-      <c r="AF40" s="145" t="n"/>
+      <c r="AD40" s="167" t="n"/>
+      <c r="AE40" s="167" t="n"/>
+      <c r="AF40" s="167" t="n"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="114" t="inlineStr">
@@ -51897,76 +51989,76 @@
       <c r="AF71" s="68" t="n"/>
     </row>
     <row r="72" ht="105" customHeight="1">
-      <c r="A72" s="143" t="inlineStr">
+      <c r="A72" s="165" t="inlineStr">
         <is>
           <t>William Stanley Jr. collection</t>
         </is>
       </c>
-      <c r="B72" s="144" t="n">
+      <c r="B72" s="166" t="n">
         <v>13282</v>
       </c>
-      <c r="C72" s="145" t="n"/>
-      <c r="D72" s="145" t="n"/>
-      <c r="E72" s="145" t="n"/>
-      <c r="F72" s="146" t="inlineStr">
+      <c r="C72" s="167" t="n"/>
+      <c r="D72" s="167" t="n"/>
+      <c r="E72" s="167" t="n"/>
+      <c r="F72" s="168" t="inlineStr">
         <is>
           <t>Correspondence regarding Stanley, Tesla and Westinghouse patents</t>
         </is>
       </c>
-      <c r="G72" s="145" t="n"/>
-      <c r="H72" s="147" t="inlineStr">
+      <c r="G72" s="167" t="n"/>
+      <c r="H72" s="169" t="inlineStr">
         <is>
           <t>Letter from Harold to Unnamed, December 16, 1952</t>
         </is>
       </c>
-      <c r="I72" s="145" t="n"/>
-      <c r="J72" s="145" t="n"/>
-      <c r="K72" s="145" t="n"/>
-      <c r="L72" s="145" t="n"/>
-      <c r="M72" s="145" t="n"/>
-      <c r="N72" s="145" t="n"/>
-      <c r="O72" s="145" t="n"/>
-      <c r="P72" s="145" t="n"/>
-      <c r="Q72" s="150" t="n">
+      <c r="I72" s="167" t="n"/>
+      <c r="J72" s="167" t="n"/>
+      <c r="K72" s="167" t="n"/>
+      <c r="L72" s="167" t="n"/>
+      <c r="M72" s="167" t="n"/>
+      <c r="N72" s="167" t="n"/>
+      <c r="O72" s="167" t="n"/>
+      <c r="P72" s="167" t="n"/>
+      <c r="Q72" s="186" t="n">
         <v>19344</v>
       </c>
-      <c r="R72" s="145" t="n"/>
-      <c r="S72" s="143" t="inlineStr">
+      <c r="R72" s="167" t="n"/>
+      <c r="S72" s="165" t="inlineStr">
         <is>
           <t xml:space="preserve">In Copyright </t>
         </is>
       </c>
-      <c r="T72" s="145" t="n"/>
-      <c r="U72" s="145" t="inlineStr">
+      <c r="T72" s="167" t="n"/>
+      <c r="U72" s="167" t="inlineStr">
         <is>
           <t>Box 7, Item 7, Item 15</t>
         </is>
       </c>
-      <c r="V72" s="147" t="inlineStr">
+      <c r="V72" s="169" t="inlineStr">
         <is>
           <t xml:space="preserve">Glass Up, Onion Paper - White paper blow </t>
         </is>
       </c>
-      <c r="W72" s="145" t="inlineStr">
+      <c r="W72" s="167" t="inlineStr">
         <is>
           <t>ZWU_SCA0319.B07.F07.15</t>
         </is>
       </c>
-      <c r="X72" s="152" t="n">
+      <c r="X72" s="172" t="n">
         <v>45504</v>
       </c>
-      <c r="Y72" s="145" t="inlineStr">
+      <c r="Y72" s="167" t="inlineStr">
         <is>
           <t>MC</t>
         </is>
       </c>
-      <c r="Z72" s="145" t="n"/>
-      <c r="AA72" s="145" t="n"/>
-      <c r="AB72" s="145" t="n"/>
-      <c r="AC72" s="141" t="n"/>
-      <c r="AD72" s="145" t="n"/>
-      <c r="AE72" s="145" t="n"/>
-      <c r="AF72" s="145" t="n"/>
+      <c r="Z72" s="167" t="n"/>
+      <c r="AA72" s="167" t="n"/>
+      <c r="AB72" s="167" t="n"/>
+      <c r="AC72" s="164" t="n"/>
+      <c r="AD72" s="167" t="n"/>
+      <c r="AE72" s="167" t="n"/>
+      <c r="AF72" s="167" t="n"/>
     </row>
     <row r="73" ht="12.75" customHeight="1">
       <c r="A73" s="68" t="n"/>

</xml_diff>